<commit_message>
Updated Excel examples in conversion
</commit_message>
<xml_diff>
--- a/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-1.xlsx
+++ b/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\00-Clients\Sparna\20-Repositories\skos-play\fr.sparna\rdf\skos\skos-play\src\main\webapp\excel_test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294AE064-0B93-4B65-B212-69B0D3737AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="27135" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -114,41 +120,41 @@
     <t>http://data.sparna.fr/vocabularies/days</t>
   </si>
   <si>
-    <t>http://data.sparna.fr/vocabularies/days#monday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#tuesday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#wednesday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#thursday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#friday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#saturday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#sunday</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#week-end</t>
-  </si>
-  <si>
-    <t>http://data.sparna.fr/vocabularies/days#saturday, http://data.sparna.fr/vocabularies/days#sunday</t>
-  </si>
-  <si>
     <t>ConceptScheme URI</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/monday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/tuesday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/wednesday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/thursday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/friday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/saturday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/sunday</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/week-end</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/vocabularies/days/saturday, http://data.sparna.fr/vocabularies/days/sunday</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -204,12 +210,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -256,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,9 +303,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,6 +355,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,26 +548,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" customWidth="1"/>
@@ -526,15 +577,15 @@
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -543,7 +594,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -552,12 +603,12 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -574,9 +625,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -588,9 +639,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -602,9 +653,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>34</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -614,9 +665,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -626,9 +677,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -640,9 +691,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -652,9 +703,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -666,9 +717,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34.5" customHeight="1">
+    <row r="15" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -677,7 +728,7 @@
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -690,12 +741,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>